<commit_message>
re-formatted and minor bug fixes.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Raul/Raul's Log.xlsx
+++ b/CLASSOPS/Raul/Raul's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="194">
   <si>
     <t>Staff Name</t>
   </si>
@@ -598,6 +598,12 @@
   </si>
   <si>
     <t xml:space="preserve">Log off PC  - pick up wireless keyboard and return to Osgoode 1014L storeroom. Log off touch screen on wall near door to storeroom. Leave mic stand and mic in room. Key for Osgoode ADR 1014 is in HNES 003 storeroom (labelled Osgoode ADR). </t>
+  </si>
+  <si>
+    <t>626</t>
+  </si>
+  <si>
+    <t>Pick up Skype camera and tripod and return to KT 516 storeroom.</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1101,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:F221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C221" sqref="C221"/>
+      <selection activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4248,6 +4254,36 @@
       </c>
       <c r="F216" s="19" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="21"/>
+      <c r="B220" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C220" s="23"/>
+      <c r="D220" s="21"/>
+      <c r="E220" s="24"/>
+      <c r="F220" s="25"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B221" s="10">
+        <v>42592</v>
+      </c>
+      <c r="C221" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D221" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E221" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F221" s="19" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Email system up and running, testing and implementation into the core system still needs to be complete.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Raul/Raul's Log.xlsx
+++ b/CLASSOPS/Raul/Raul's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3128" uniqueCount="434">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1321,6 +1321,9 @@
   </si>
   <si>
     <t>Pick up one audience handheld mic  and stands and return to rear booth. Leave podium mic  and desk mics in place</t>
+  </si>
+  <si>
+    <t>INC000000739935</t>
   </si>
 </sst>
 </file>
@@ -1813,10 +1816,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F895"/>
+  <dimension ref="A1:F897"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A881" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E900" sqref="E900"/>
+    <sheetView tabSelected="1" topLeftCell="A875" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F902" sqref="F902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14193,6 +14196,46 @@
       </c>
       <c r="E895" s="6" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A896" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B896" s="5">
+        <v>42676</v>
+      </c>
+      <c r="C896" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D896" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E896" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F896" s="14" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A897" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B897" s="5">
+        <v>42676</v>
+      </c>
+      <c r="C897" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D897" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E897" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F897" s="14" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>